<commit_message>
Added results utlising 1 to 8 cores on a function
</commit_message>
<xml_diff>
--- a/TimeRecord.xlsx
+++ b/TimeRecord.xlsx
@@ -8,13 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pstanis/personal_projects/multiprocessing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFA74DC0-0BAE-3049-94FE-E468085396F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5594BFB1-FFEC-FB4F-B354-25F31CB15221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="17280" windowHeight="21580" xr2:uid="{0B376BBB-F0E9-B940-A34F-E1CBB3CA6477}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v2.0" hidden="1">Sheet1!$D$2</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">Sheet1!$D$3:$D$6</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">Sheet1!$E$2</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">Sheet1!$E$3:$E$6</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Number of Processes</t>
   </si>
@@ -44,13 +50,46 @@
     <t>Time to execute</t>
   </si>
   <si>
-    <t>Number of threads</t>
+    <t>Time to execute (s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normal run </t>
+  </si>
+  <si>
+    <t>Number of runs</t>
+  </si>
+  <si>
+    <t>0.16s</t>
+  </si>
+  <si>
+    <t>1.27s</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Multiprocessing 8 runs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slight overhead in running process which is why it's longer than the normal run </t>
+  </si>
+  <si>
+    <t>Multithreading 8 runs</t>
+  </si>
+  <si>
+    <t>Threads</t>
+  </si>
+  <si>
+    <t>We run a function once, and then 8 times to see how it affects the run time of a CPU heavy task. We can then showcase how 8 pooled processes can do 8 runs in a similar time to just one run. Threading however has no affect in this case, as the GIL prevents more than one thread doing something at one time.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0000000000E+00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -80,8 +119,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -97,6 +140,878 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time to execute (s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$3:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$3:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000000000E+00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D625-2445-9EED-6619A886E5D4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="507744240"/>
+        <c:axId val="507746784"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="507744240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="507746784"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="507746784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000000000E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="507744240"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>187364</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>141112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>713394</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1790388</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E732553D-C8A5-A05F-F942-8103CCBD12F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -396,35 +1311,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2DF814A-5D21-1A4B-9268-DB166B5752B5}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.1640625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.83203125" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
+      <c r="E4" s="1">
+        <v>0.69</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" ht="153" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>